<commit_message>
Fixed bug geek arrow rotation
</commit_message>
<xml_diff>
--- a/Document/Issues.xlsx
+++ b/Document/Issues.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,13 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>胖子只有落地才应该调用旋转的飞行姿势</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>胖子被打的动作方向应该朝向飞行方向，并随飞行方向改变</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,7 +92,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -126,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -161,7 +169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -381,14 +389,20 @@
     <col min="1" max="1" width="92.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>